<commit_message>
Added final report, edited figures
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicoline L. Thomsen\Documents\1. GitHub Repos\EmbodiedAI_21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852E1F8E-1AAE-41D8-84CF-47A1037EBEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B5B4DE-0F0E-4F75-9620-C71D5F228BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="15" windowWidth="16178" windowHeight="12743" xr2:uid="{0C90D040-E91F-4C0C-903A-353C68E5954F}"/>
+    <workbookView xWindow="-21810" yWindow="1755" windowWidth="19365" windowHeight="13005" xr2:uid="{0C90D040-E91F-4C0C-903A-353C68E5954F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>Straight</t>
   </si>
@@ -84,7 +84,13 @@
     <t>Change to see black on the other sensor when sharp_turn</t>
   </si>
   <si>
-    <t>WITH ANGLE</t>
+    <t>Success %</t>
+  </si>
+  <si>
+    <t>WITHOUT CAN</t>
+  </si>
+  <si>
+    <t>WITHOUT CAN AND WITH ANGLE</t>
   </si>
 </sst>
 </file>
@@ -108,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -116,12 +122,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,52 +452,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E12C40A-319E-4B0A-AD0B-2D100FA0D760}">
-  <dimension ref="B1:U49"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="I14" sqref="H3:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
       </c>
       <c r="N2" t="s">
         <v>4</v>
@@ -490,33 +482,33 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
       </c>
       <c r="N3" t="s">
         <v>0</v>
@@ -533,17 +525,8 @@
       <c r="R3" t="s">
         <v>3</v>
       </c>
-      <c r="S3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T3" t="s">
-        <v>7</v>
-      </c>
-      <c r="U3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -557,7 +540,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -587,7 +570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
@@ -631,7 +614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
@@ -642,7 +625,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -675,7 +658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1</v>
       </c>
@@ -686,7 +669,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -719,7 +702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1</v>
       </c>
@@ -763,7 +746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1</v>
       </c>
@@ -807,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1</v>
       </c>
@@ -851,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>1</v>
       </c>
@@ -895,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>1</v>
       </c>
@@ -909,7 +892,7 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -939,7 +922,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
       <c r="N13">
         <v>1</v>
       </c>
@@ -956,20 +966,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B17" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <f>100*SUM(B4:B13)/10</f>
+        <v>100</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" ref="C14:J14" si="0">100*SUM(C4:C13)/10</f>
+        <v>100</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N14" s="1">
+        <f>100*SUM(N4:N13)/10</f>
+        <v>100</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" ref="O14" si="1">100*SUM(O4:O13)/10</f>
+        <v>60</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" ref="P14" si="2">100*SUM(P4:P13)/10</f>
+        <v>80</v>
+      </c>
+      <c r="Q14" s="1">
+        <f t="shared" ref="Q14:R14" si="3">100*SUM(Q4:Q13)/10</f>
+        <v>100</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>4</v>
       </c>
       <c r="G18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="N18" t="s">
+        <v>9</v>
+      </c>
+      <c r="P18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>0</v>
       </c>
@@ -997,8 +1077,20 @@
       <c r="J19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="N19" t="s">
+        <v>10</v>
+      </c>
+      <c r="O19" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>1</v>
       </c>
@@ -1026,8 +1118,20 @@
       <c r="J20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>1</v>
       </c>
@@ -1055,8 +1159,20 @@
       <c r="J21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>1</v>
       </c>
@@ -1084,8 +1200,20 @@
       <c r="J22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>1</v>
       </c>
@@ -1113,8 +1241,20 @@
       <c r="J23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>1</v>
       </c>
@@ -1142,8 +1282,20 @@
       <c r="J24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>1</v>
       </c>
@@ -1171,304 +1323,246 @@
       <c r="J25">
         <v>0</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="1">
+        <f>100*SUM(B20:B29)/10</f>
+        <v>100</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" ref="C30" si="4">100*SUM(C20:C29)/10</f>
+        <v>60</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" ref="D30" si="5">100*SUM(D20:D29)/10</f>
+        <v>90</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" ref="E30" si="6">100*SUM(E20:E29)/10</f>
+        <v>60</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" ref="F30" si="7">100*SUM(F20:F29)/10</f>
+        <v>100</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" ref="G30" si="8">100*SUM(G20:G29)/10</f>
+        <v>100</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" ref="H30" si="9">100*SUM(H20:H29)/10</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" ref="I30" si="10">100*SUM(I20:I29)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" ref="J30" si="11">100*SUM(J20:J29)/10</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="1">
+        <f>100*SUM(N20:N29)/10</f>
+        <v>100</v>
+      </c>
+      <c r="O30" s="1">
+        <f t="shared" ref="O30" si="12">100*SUM(O20:O29)/10</f>
+        <v>70</v>
+      </c>
+      <c r="P30" s="1">
+        <f t="shared" ref="P30" si="13">100*SUM(P20:P29)/10</f>
+        <v>70</v>
+      </c>
+      <c r="Q30" s="1">
+        <f t="shared" ref="Q30" si="14">100*SUM(Q20:Q29)/10</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B36" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B37" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" t="s">
-        <v>13</v>
-      </c>
-      <c r="E37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B49">
-        <f>SUM(B38:B47)/10</f>
-        <v>1</v>
-      </c>
-      <c r="C49">
-        <f>SUM(C38:C47)/10</f>
-        <v>0.7</v>
-      </c>
-      <c r="D49">
-        <f>SUM(D38:D47)/10</f>
-        <v>0.7</v>
-      </c>
-      <c r="E49">
-        <f>SUM(E38:E47)/10</f>
-        <v>0.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>